<commit_message>
Updated draft S-158:102 0.1.0
</commit_message>
<xml_diff>
--- a/Documents/S-158-102/0.1.0/S-158_102_0_1_0_20241015.xlsx
+++ b/Documents/S-158-102/0.1.0/S-158_102_0_1_0_20241015.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\git\S-100-Validation-Checks\Documents\S-158-102\0.1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6BB010-E6C8-474D-A2D7-68A40B5ACAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AA4196-8CEF-4DE1-9570-07E36C75CDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="18240" activeTab="1" xr2:uid="{D500D42E-56ED-44C2-B321-3F3845968AA3}"/>
   </bookViews>
@@ -3352,8 +3352,8 @@
   <dimension ref="A1:Q454"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>